<commit_message>
:hammer: Colagem dos nomes
Ajustando a copia e colagem dos nomes dos alunos para que todas as carteirinhas do modelo sejam preenchidas corretamente
</commit_message>
<xml_diff>
--- a/CarterinhasPreenchidas.xlsx
+++ b/CarterinhasPreenchidas.xlsx
@@ -3190,7 +3190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:N386"/>
+  <dimension ref="B2:N280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:G17"/>
@@ -3321,6 +3321,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Rayssa Lorena de Souza do Amaral</t>
+        </is>
+      </c>
       <c r="N8" s="20" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1" s="19">
@@ -3511,6 +3516,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Arthur Corrêa de Souza</t>
+        </is>
+      </c>
       <c r="G22" s="20" t="n"/>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -3519,7 +3529,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Arthur Corrêa de Souza</t>
+          <t>Renan Henrique da Silva Constantino</t>
         </is>
       </c>
       <c r="N22" s="20" t="n"/>
@@ -3712,6 +3722,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Dhiarlley Santos Ramos</t>
+        </is>
+      </c>
       <c r="G36" s="20" t="n"/>
       <c r="I36" s="9" t="inlineStr">
         <is>
@@ -3720,7 +3735,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Dhiarlley Santos Ramos</t>
+          <t>Samuel Alencar Felix</t>
         </is>
       </c>
       <c r="N36" s="20" t="n"/>
@@ -3914,6 +3929,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Emanuelly Vitória dos Santos Silva</t>
+        </is>
+      </c>
       <c r="G50" s="20" t="n"/>
       <c r="I50" s="9" t="inlineStr">
         <is>
@@ -3922,7 +3942,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Emanuelly Vitória dos Santos Silva</t>
+          <t>Valentina Bispo Santana</t>
         </is>
       </c>
       <c r="N50" s="20" t="n"/>
@@ -4115,6 +4135,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Gabriel Pereira Silva Fadeli</t>
+        </is>
+      </c>
       <c r="G64" s="20" t="n"/>
       <c r="I64" s="9" t="inlineStr">
         <is>
@@ -4123,7 +4148,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Gabriel Pereira Silva Fadeli</t>
+          <t>Vinícius da Silva Nichel</t>
         </is>
       </c>
       <c r="N64" s="20" t="n"/>
@@ -4317,6 +4342,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Giulia Amanayara Ribeiro Reis</t>
+        </is>
+      </c>
       <c r="G78" s="20" t="n"/>
       <c r="I78" s="9" t="inlineStr">
         <is>
@@ -4325,7 +4355,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Giulia Amanayara Ribeiro Reis</t>
+          <t>Heitor Andrade Ferreira dos Santos</t>
         </is>
       </c>
       <c r="N78" s="20" t="n"/>
@@ -4518,6 +4548,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Heitor Henrique Alves Santos</t>
+        </is>
+      </c>
       <c r="G92" s="20" t="n"/>
       <c r="I92" s="9" t="inlineStr">
         <is>
@@ -4526,7 +4561,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Heitor Henrique Alves Santos</t>
+          <t>Brenda Mikaelly Castro Pimentel</t>
         </is>
       </c>
       <c r="N92" s="20" t="n"/>
@@ -4720,6 +4755,11 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Heitor Natanael Santos de Oliveira</t>
+        </is>
+      </c>
       <c r="G106" s="20" t="n"/>
       <c r="I106" s="9" t="inlineStr">
         <is>
@@ -4728,7 +4768,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Heitor Natanael Santos de Oliveira</t>
+          <t>Raylan Canuto Peixoto</t>
         </is>
       </c>
       <c r="N106" s="20" t="n"/>
@@ -4921,15 +4961,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Heitor Santos Aguado</t>
+        </is>
+      </c>
       <c r="G120" s="20" t="n"/>
       <c r="I120" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J120" t="inlineStr">
-        <is>
-          <t>Heitor Santos Aguado</t>
         </is>
       </c>
       <c r="N120" s="20" t="n"/>
@@ -5123,15 +5163,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Henry Lucca Alves Aguiar</t>
+        </is>
+      </c>
       <c r="G134" s="20" t="n"/>
       <c r="I134" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J134" t="inlineStr">
-        <is>
-          <t>Henry Lucca Alves Aguiar</t>
         </is>
       </c>
       <c r="N134" s="20" t="n"/>
@@ -5324,15 +5364,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Jean Arthur da Silva Azevedo</t>
+        </is>
+      </c>
       <c r="G148" s="20" t="n"/>
       <c r="I148" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J148" t="inlineStr">
-        <is>
-          <t>Jean Arthur da Silva Azevedo</t>
         </is>
       </c>
       <c r="N148" s="20" t="n"/>
@@ -5526,15 +5566,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Kauâ Lucca Alves dos Santos</t>
+        </is>
+      </c>
       <c r="G162" s="20" t="n"/>
       <c r="I162" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J162" t="inlineStr">
-        <is>
-          <t>Kauâ Lucca Alves dos Santos</t>
         </is>
       </c>
       <c r="N162" s="20" t="n"/>
@@ -5727,15 +5767,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Laryssa de Jesus Rodrigues</t>
+        </is>
+      </c>
       <c r="G176" s="20" t="n"/>
       <c r="I176" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J176" t="inlineStr">
-        <is>
-          <t>Laryssa de Jesus Rodrigues</t>
         </is>
       </c>
       <c r="N176" s="20" t="n"/>
@@ -5929,15 +5969,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Laura Isabelly Santos Vieira</t>
+        </is>
+      </c>
       <c r="G190" s="20" t="n"/>
       <c r="I190" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J190" t="inlineStr">
-        <is>
-          <t>Laura Isabelly Santos Vieira</t>
         </is>
       </c>
       <c r="N190" s="20" t="n"/>
@@ -6130,15 +6170,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Lívia dos Santos Capodeferro</t>
+        </is>
+      </c>
       <c r="G204" s="20" t="n"/>
       <c r="I204" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J204" t="inlineStr">
-        <is>
-          <t>Lívia dos Santos Capodeferro</t>
         </is>
       </c>
       <c r="N204" s="20" t="n"/>
@@ -6332,15 +6372,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Miguel Marçal de Oliveira</t>
+        </is>
+      </c>
       <c r="G218" s="20" t="n"/>
       <c r="I218" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J218" t="inlineStr">
-        <is>
-          <t>Miguel Marçal de Oliveira</t>
         </is>
       </c>
       <c r="N218" s="20" t="n"/>
@@ -6533,15 +6573,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Nathan Souza Martins</t>
+        </is>
+      </c>
       <c r="G232" s="20" t="n"/>
       <c r="I232" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J232" t="inlineStr">
-        <is>
-          <t>Nathan Souza Martins</t>
         </is>
       </c>
       <c r="N232" s="20" t="n"/>
@@ -6735,16 +6775,16 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Neudismar Stephia de Los Angeles
+Cermeño Guzman</t>
+        </is>
+      </c>
       <c r="G246" s="20" t="n"/>
       <c r="I246" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J246" t="inlineStr">
-        <is>
-          <t>Neudismar Stephia de Los Angeles
-Cermeño Guzman</t>
         </is>
       </c>
       <c r="N246" s="20" t="n"/>
@@ -6937,15 +6977,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Pedro da Silva Alexandre</t>
+        </is>
+      </c>
       <c r="G260" s="20" t="n"/>
       <c r="I260" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J260" t="inlineStr">
-        <is>
-          <t>Pedro da Silva Alexandre</t>
         </is>
       </c>
       <c r="N260" s="20" t="n"/>
@@ -7139,15 +7179,15 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Pedro Henrique Cassiano Machado</t>
+        </is>
+      </c>
       <c r="G274" s="20" t="n"/>
       <c r="I274" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="J274" t="inlineStr">
-        <is>
-          <t>Pedro Henrique Cassiano Machado</t>
         </is>
       </c>
       <c r="N274" s="20" t="n"/>
@@ -7241,62 +7281,6 @@
       <c r="L280" s="1" t="n"/>
       <c r="M280" s="1" t="n"/>
       <c r="N280" s="13" t="n"/>
-    </row>
-    <row r="288">
-      <c r="J288" t="inlineStr">
-        <is>
-          <t>Rayssa Lorena de Souza do Amaral</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="J302" t="inlineStr">
-        <is>
-          <t>Renan Henrique da Silva Constantino</t>
-        </is>
-      </c>
-    </row>
-    <row r="316">
-      <c r="J316" t="inlineStr">
-        <is>
-          <t>Samuel Alencar Felix</t>
-        </is>
-      </c>
-    </row>
-    <row r="330">
-      <c r="J330" t="inlineStr">
-        <is>
-          <t>Valentina Bispo Santana</t>
-        </is>
-      </c>
-    </row>
-    <row r="344">
-      <c r="J344" t="inlineStr">
-        <is>
-          <t>Vinícius da Silva Nichel</t>
-        </is>
-      </c>
-    </row>
-    <row r="358">
-      <c r="J358" t="inlineStr">
-        <is>
-          <t>Heitor Andrade Ferreira dos Santos</t>
-        </is>
-      </c>
-    </row>
-    <row r="372">
-      <c r="J372" t="inlineStr">
-        <is>
-          <t>Brenda Mikaelly Castro Pimentel</t>
-        </is>
-      </c>
-    </row>
-    <row r="386">
-      <c r="J386" t="inlineStr">
-        <is>
-          <t>Raylan Canuto Peixoto</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="250">

</xml_diff>